<commit_message>
added diagrams, changed age grps
</commit_message>
<xml_diff>
--- a/data/codebooks/codebook_values.xlsx
+++ b/data/codebooks/codebook_values.xlsx
@@ -517,13 +517,13 @@
     <t>02 bis 5 Jahre</t>
   </si>
   <si>
-    <t>&lt;5 years</t>
+    <t>02 to 05 years</t>
   </si>
   <si>
     <t>06 bis 9 Jahre</t>
   </si>
   <si>
-    <t>6 to 9 years</t>
+    <t>06 to 09 years</t>
   </si>
   <si>
     <t>10 bis 14 Jahre</t>
@@ -541,7 +541,7 @@
     <t>18+ Jahre</t>
   </si>
   <si>
-    <t>&gt;18 years</t>
+    <t>18+ years</t>
   </si>
   <si>
     <t>[05.09]</t>
@@ -1512,7 +1512,7 @@
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
@@ -1542,7 +1542,7 @@
       </c>
       <c r="E14" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="E15" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1572,7 +1572,7 @@
       </c>
       <c r="E16" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="E17" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="E18" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="E19" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="33">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="31.5">
       <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="E20" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="E21" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
@@ -1660,7 +1660,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="30.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="25.5">
       <c r="A23" s="5" t="s">
         <v>53</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="5" t="s">
         <v>53</v>
       </c>
@@ -1692,7 +1692,7 @@
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="5" t="s">
         <v>53</v>
       </c>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="E25" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="30.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="5" t="s">
         <v>53</v>
       </c>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="E26" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="30.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="5" t="s">
         <v>53</v>
       </c>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="E27" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="5" t="s">
         <v>53</v>
       </c>
@@ -1752,7 +1752,7 @@
       </c>
       <c r="E28" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="30.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="5" t="s">
         <v>53</v>
       </c>
@@ -1767,7 +1767,7 @@
       </c>
       <c r="E29" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="5" t="s">
         <v>53</v>
       </c>
@@ -1782,7 +1782,7 @@
       </c>
       <c r="E30" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="30.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1" t="s">
         <v>73</v>
       </c>
@@ -1795,7 +1795,7 @@
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="30.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="5" t="s">
         <v>73</v>
       </c>

</xml_diff>